<commit_message>
Added PCB production files
Gerbers, drill, centroid, fab readme, PCB BOM. Reviewed and added PCB
tag number to top level BOM
</commit_message>
<xml_diff>
--- a/POSCON.BOM.xlsx
+++ b/POSCON.BOM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="0" windowWidth="28260" windowHeight="19540" tabRatio="500"/>
+    <workbookView xWindow="4440" yWindow="0" windowWidth="28260" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>Product Name:</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>POSCON.v1.0</t>
-  </si>
-  <si>
-    <t>Tag:</t>
   </si>
   <si>
     <t>POSCON.BACK</t>
@@ -182,6 +179,12 @@
   </si>
   <si>
     <t>http://sonicmfg.com/</t>
+  </si>
+  <si>
+    <t>v1.0</t>
+  </si>
+  <si>
+    <t>Tag title:</t>
   </si>
 </sst>
 </file>
@@ -326,6 +329,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -651,25 +659,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P50"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" customWidth="1"/>
+    <col min="1" max="1" width="7.125" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="41.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41.375" customWidth="1"/>
+    <col min="4" max="4" width="26.125" customWidth="1"/>
+    <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.125" customWidth="1"/>
+    <col min="8" max="8" width="96" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16">
+    <row r="1" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +688,7 @@
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>36</v>
@@ -689,7 +699,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="16">
+    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -709,7 +719,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="16">
+    <row r="3" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -725,7 +735,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="16">
+    <row r="4" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -737,7 +747,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="16">
+    <row r="5" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -749,7 +759,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
@@ -776,463 +786,462 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="16">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+    <row r="7" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>1</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="12"/>
       <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="16">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="G7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>2</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="12"/>
       <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="2"/>
+      <c r="G8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="16">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+    <row r="9" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>1</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="2"/>
+      <c r="G9" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="16">
+    <row r="10" spans="1:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>1</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>11</v>
+      <c r="B10" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="J10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="30">
+      <c r="G10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="14"/>
       <c r="G11" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="16">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+    <row r="12" spans="1:11" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>2</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="E12" s="12"/>
       <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="2"/>
+      <c r="G12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="16">
+    <row r="13" spans="1:11" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>32</v>
+        <v>45</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="14"/>
-      <c r="G13" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>53</v>
+      <c r="G13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="16">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+    <row r="14" spans="1:11" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>2</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>30</v>
+      </c>
       <c r="E14" s="12"/>
       <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="2"/>
+      <c r="G14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="30">
-      <c r="A15" s="12">
-        <v>1</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="12"/>
+    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="14"/>
-      <c r="G15" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" ht="30">
-      <c r="A16" s="12">
-        <v>1</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="12"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="14"/>
-      <c r="G16" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:16" ht="45">
-      <c r="A17" s="12">
-        <v>2</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="12"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="14"/>
-      <c r="G17" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:16" ht="45">
-      <c r="A18" s="12">
-        <v>2</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="12"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="14"/>
-      <c r="G18" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:16" ht="30">
-      <c r="A19" s="12">
-        <v>2</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="12"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="14"/>
-      <c r="G19" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:16" ht="16">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="F20" s="12"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="2"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="7"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:16" ht="16">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+    <row r="21" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="12"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="12"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:16" ht="16">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="F22" s="12"/>
       <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:16" ht="16">
-      <c r="B23" s="13"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:16" ht="16">
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="1:16" ht="16">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="7"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="1:16" ht="16">
-      <c r="B26" s="12"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="2"/>
-    </row>
-    <row r="27" spans="1:16" ht="16">
-      <c r="B27" s="12"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-    </row>
-    <row r="28" spans="1:16" ht="16">
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-    </row>
-    <row r="29" spans="1:16" ht="16">
+    </row>
+    <row r="29" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-    </row>
-    <row r="30" spans="1:16" ht="16">
+    </row>
+    <row r="30" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-    </row>
-    <row r="31" spans="1:16" ht="16">
+    </row>
+    <row r="31" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:16" ht="16">
+    <row r="32" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="2:16" ht="16">
+    <row r="33" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="2:16" ht="16">
+    <row r="34" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="2:16" ht="16">
+    <row r="35" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="2:16" ht="16">
+    <row r="36" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="2:16" ht="16">
-      <c r="B37" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+    </row>
+    <row r="37" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="2:16" ht="16">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="2:16" ht="16">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="2:16" ht="16">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="2:16" ht="16">
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="2:16" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="2:16" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1249,8 +1258,8 @@
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
     </row>
-    <row r="42" spans="2:16" ht="16">
-      <c r="B42" s="1"/>
+    <row r="42" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1266,115 +1275,64 @@
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
     </row>
-    <row r="43" spans="2:16">
-      <c r="B43" s="3"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" spans="2:16" ht="16">
-      <c r="B44" s="3"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="2:16" ht="16">
-      <c r="B45" s="3"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" spans="2:16" ht="16">
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-    </row>
-    <row r="47" spans="2:16" ht="16">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
-    </row>
-    <row r="48" spans="2:16" ht="16">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-    </row>
-    <row r="49" spans="2:16" ht="16">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-    </row>
-    <row r="50" spans="2:16" ht="16">
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
+    <row r="43" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+    </row>
+    <row r="44" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+    </row>
+    <row r="45" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H11" r:id="rId1" location="90272a110/=tmwrzh"/>
-    <hyperlink ref="H17" r:id="rId2" location="93580a220/=txsdeu"/>
-    <hyperlink ref="H18" r:id="rId3" location="3225t3/=ta5mtv"/>
-    <hyperlink ref="H19" r:id="rId4" location="90480a009/=ta5u6v"/>
+    <hyperlink ref="H8" r:id="rId1" location="90272a110/=tmwrzh"/>
+    <hyperlink ref="H12" r:id="rId2" location="93580a220/=txsdeu"/>
+    <hyperlink ref="H13" r:id="rId3" location="3225t3/=ta5mtv"/>
+    <hyperlink ref="H14" r:id="rId4" location="90480a009/=ta5u6v"/>
+    <hyperlink ref="H10" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Updated Backplate Stud Size
Changed stud size from 6-32 to 8-32
</commit_message>
<xml_diff>
--- a/POSCON.BOM.xlsx
+++ b/POSCON.BOM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="0" windowWidth="28260" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="36260" yWindow="360" windowWidth="28260" windowHeight="19540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>Product Name:</t>
   </si>
@@ -27,6 +27,12 @@
     <t>Product Number:</t>
   </si>
   <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Last Updated:</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -81,13 +87,28 @@
     <t>1/8" Aluminum Plate</t>
   </si>
   <si>
+    <t>J+M Manufacturing</t>
+  </si>
+  <si>
     <t>Press-in Studs</t>
   </si>
   <si>
-    <t>93580A220</t>
-  </si>
-  <si>
-    <t>http://www.mcmaster.com/#93580a220/=txsdeu</t>
+    <t>Pipe Clamps</t>
+  </si>
+  <si>
+    <t>3225T3</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#3225t3/=ta5mtv</t>
+  </si>
+  <si>
+    <t>Nuts</t>
+  </si>
+  <si>
+    <t>90480A009</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#90480a009/=ta5u6v</t>
   </si>
   <si>
     <t>POSCON.PCB</t>
@@ -96,6 +117,9 @@
     <t>POSCON</t>
   </si>
   <si>
+    <t>Position Controller Gen3</t>
+  </si>
+  <si>
     <t>Tag</t>
   </si>
   <si>
@@ -114,6 +138,9 @@
     <t>Injection Molded Serpac Part</t>
   </si>
   <si>
+    <t>Sonic</t>
+  </si>
+  <si>
     <t>U-Line</t>
   </si>
   <si>
@@ -123,29 +150,38 @@
     <t>Pre-Cut Double-Sided Foam Squares 1" x 1" x 1/32"</t>
   </si>
   <si>
+    <t>Rubber-Cushioned Loop Clamp, Zinc-Plated Steel, EPDM Cushion, for 3/8" Outside Diameter</t>
+  </si>
+  <si>
+    <t>Zinc-Plated Steel Machine Screw Hex Nut, 8-32 Thread Size, 11/32" Width, 1/8" Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serpac </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PCB</t>
+  </si>
+  <si>
+    <t>http://www.jmmfg.com/</t>
+  </si>
+  <si>
+    <t>http://sonicmfg.com/</t>
+  </si>
+  <si>
+    <t>http://www.serpac.com/,  OEM Part No. RB221TC</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#93580a420/=u5yq8a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t>93580A420</t>
+  </si>
+  <si>
     <t>"PEM® Press-in Stud
-Type 18-8 Stainless Steel, 6-32 Thread, 1/2"" Long, Number Fhs632-8"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serpac </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PCB</t>
-  </si>
-  <si>
-    <t>http://www.serpac.com/,  OEM Part No. RB221TC</t>
-  </si>
-  <si>
-    <t>New Position Controller</t>
-  </si>
-  <si>
-    <t>Date Released:</t>
-  </si>
-  <si>
-    <t>POSCON.MECH.v1.0</t>
-  </si>
-  <si>
-    <t>POSCON.PCB.v1.0</t>
+Type 18-8 Stainless Steel, 8-32 Thread, 1/2"" Long, Number Fhs632-8"</t>
   </si>
 </sst>
 </file>
@@ -155,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -230,38 +266,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -285,11 +289,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
@@ -323,22 +328,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -347,11 +336,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -679,451 +663,477 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.125" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="41.375" customWidth="1"/>
-    <col min="4" max="4" width="26.125" customWidth="1"/>
-    <col min="5" max="5" width="24.125" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.125" customWidth="1"/>
-    <col min="8" max="8" width="102.875" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="8" max="8" width="102.83203125" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:11" ht="16">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="1:11" ht="16">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="21">
-        <v>41926</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>41848</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+    <row r="3" spans="1:11" ht="16">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>41925</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+    <row r="4" spans="1:11" ht="16">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
+    <row r="5" spans="1:11" ht="16">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:11">
+      <c r="A6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="E6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" ht="16">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="16">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="16">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" ht="16">
+      <c r="A10" s="12">
+        <v>1</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" ht="30">
+      <c r="A11" s="12">
         <v>2</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="22" t="s">
+      <c r="B11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="16">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" ht="16">
+      <c r="A13" s="12">
+        <v>1</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" ht="16">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" ht="30">
+      <c r="A15" s="12">
+        <v>1</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" ht="30">
+      <c r="A16" s="12">
+        <v>1</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" ht="45">
+      <c r="A17" s="12">
+        <v>2</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:16" ht="45">
+      <c r="A18" s="12">
+        <v>2</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
-        <v>1</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="23" t="s">
+      <c r="E18" s="12"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" ht="30">
+      <c r="A19" s="12">
+        <v>2</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
-        <v>2</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
-        <v>1</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="23">
-        <v>1</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="23">
-        <v>1</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:16" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="23">
-        <v>2</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="6"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
+    <row r="20" spans="1:16" ht="16">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
+    <row r="21" spans="1:16" ht="16">
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
+    <row r="22" spans="1:16" ht="16">
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
+    <row r="23" spans="1:16" ht="16">
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
+    <row r="24" spans="1:16" ht="16">
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="6"/>
+    <row r="25" spans="1:16" ht="16">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="7"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="6"/>
+    <row r="26" spans="1:16" ht="16">
+      <c r="B26" s="12"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="7"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="11"/>
+    <row r="27" spans="1:16" ht="16">
+      <c r="B27" s="12"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="12"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
     </row>
-    <row r="28" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="16">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1137,7 +1147,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="16">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1154,7 +1164,7 @@
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
     </row>
-    <row r="30" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="16">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1171,67 +1181,67 @@
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
     </row>
-    <row r="31" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="16">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="16">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" ht="16">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" ht="16">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" ht="16">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" ht="16">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" ht="16">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" ht="16">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" ht="16">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" ht="16">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" ht="16">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1248,7 +1258,7 @@
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
     </row>
-    <row r="42" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" ht="16">
       <c r="B42" s="1"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1265,25 +1275,25 @@
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16">
       <c r="B43" s="3"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="2:16" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C43" s="8"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="2:16" ht="16">
       <c r="B44" s="3"/>
-      <c r="C44" s="8"/>
+      <c r="C44" s="9"/>
       <c r="D44" s="3"/>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="2:16" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="2:16" ht="16">
       <c r="B45" s="3"/>
-      <c r="C45" s="8"/>
+      <c r="C45" s="9"/>
       <c r="D45" s="3"/>
-      <c r="E45" s="9"/>
-    </row>
-    <row r="46" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="E45" s="10"/>
+    </row>
+    <row r="46" spans="2:16" ht="16">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1300,7 +1310,7 @@
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
     </row>
-    <row r="47" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:16" ht="16">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -1317,7 +1327,7 @@
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
     </row>
-    <row r="48" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:16" ht="16">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -1334,7 +1344,7 @@
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
     </row>
-    <row r="49" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:16" ht="16">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -1351,7 +1361,7 @@
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
     </row>
-    <row r="50" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:16" ht="16">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -1371,10 +1381,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H11" r:id="rId1" location="90272a110/=tmwrzh"/>
-    <hyperlink ref="H17" r:id="rId2" location="93580a220/=txsdeu"/>
+    <hyperlink ref="H17" r:id="rId2" location="93580a420/=u5yq8a"/>
+    <hyperlink ref="H18" r:id="rId3" location="3225t3/=ta5mtv"/>
+    <hyperlink ref="H19" r:id="rId4" location="90480a009/=ta5u6v"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Moved faceplate mounting screws to top level BOM
</commit_message>
<xml_diff>
--- a/POSCON.BOM.xlsx
+++ b/POSCON.BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Product Name:</t>
   </si>
@@ -86,6 +86,29 @@
   </si>
   <si>
     <t>http://sonicmfg.com/</t>
+  </si>
+  <si>
+    <t>Faceplate Mounting Screws</t>
+  </si>
+  <si>
+    <t>18-8 Stainless Steel Pan Head Phillips Machine Screw 4-40 thread, 9/16“ Length</t>
+  </si>
+  <si>
+    <t>91772A111</t>
+  </si>
+  <si>
+    <t>McMaster-Carr</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>http://www.mcmaster.com/#91772a111/=wy8q26</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">     </t>
@@ -98,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -139,6 +162,12 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12"/>
@@ -188,7 +217,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -196,51 +225,39 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="10" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1504,7 +1521,7 @@
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="5.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.3672" style="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.625" style="1" customWidth="1"/>
@@ -1537,33 +1554,33 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" ht="16.5" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" t="s" s="8">
         <v>5</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="9">
         <v>42129</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" ht="16.5" customHeight="1">
       <c r="A3" s="2"/>
@@ -1573,16 +1590,16 @@
       <c r="E3" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="9">
         <v>42129</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
     </row>
     <row r="4" ht="16.5" customHeight="1">
       <c r="A4" s="2"/>
@@ -1594,10 +1611,10 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
     </row>
     <row r="5" ht="16.5" customHeight="1">
       <c r="A5" s="2"/>
@@ -1609,339 +1626,354 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
     </row>
     <row r="6" ht="19" customHeight="1">
-      <c r="A6" t="s" s="8">
+      <c r="A6" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="B6" t="s" s="8">
+      <c r="B6" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="C6" t="s" s="8">
+      <c r="C6" t="s" s="3">
         <v>10</v>
       </c>
-      <c r="D6" t="s" s="8">
+      <c r="D6" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="E6" t="s" s="8">
+      <c r="E6" t="s" s="3">
         <v>12</v>
       </c>
-      <c r="F6" t="s" s="8">
+      <c r="F6" t="s" s="3">
         <v>13</v>
       </c>
-      <c r="G6" t="s" s="8">
+      <c r="G6" t="s" s="3">
         <v>14</v>
       </c>
       <c r="H6" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" ht="16.5" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" ht="16.5" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" ht="16.5" customHeight="1">
-      <c r="A9" s="10">
+      <c r="A9" s="4">
         <v>1</v>
       </c>
-      <c r="B9" t="s" s="12">
+      <c r="B9" t="s" s="8">
         <v>16</v>
       </c>
-      <c r="C9" t="s" s="12">
+      <c r="C9" t="s" s="8">
         <v>17</v>
       </c>
-      <c r="D9" t="s" s="12">
+      <c r="D9" t="s" s="8">
         <v>16</v>
       </c>
-      <c r="E9" t="s" s="12">
+      <c r="E9" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
     </row>
     <row r="10" ht="16.5" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
     </row>
     <row r="11" ht="30.75" customHeight="1">
-      <c r="A11" s="14">
+      <c r="A11" s="5">
         <v>1</v>
       </c>
-      <c r="B11" t="s" s="14">
+      <c r="B11" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="C11" t="s" s="14">
+      <c r="C11" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="D11" t="s" s="12">
+      <c r="D11" t="s" s="8">
         <v>21</v>
       </c>
-      <c r="E11" t="s" s="14">
+      <c r="E11" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" t="s" s="12">
+      <c r="F11" s="4"/>
+      <c r="G11" t="s" s="8">
         <v>23</v>
       </c>
-      <c r="H11" t="s" s="6">
+      <c r="H11" t="s" s="8">
         <v>24</v>
       </c>
       <c r="I11" s="4"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" ht="16.5" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="13" ht="16.5" customHeight="1">
-      <c r="A13" s="2"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
+      <c r="A13" s="4">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s" s="8">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" t="s" s="8">
+        <v>28</v>
+      </c>
+      <c r="H13" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" ht="16.5" customHeight="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" t="s" s="12">
-        <v>25</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" ht="16.5" customHeight="1">
       <c r="A15" s="2"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" ht="16.5" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" ht="16.5" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
     </row>
     <row r="18" ht="16.5" customHeight="1">
       <c r="A18" s="2"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
     </row>
     <row r="19" ht="16.5" customHeight="1">
       <c r="A19" s="2"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="4"/>
     </row>
     <row r="20" ht="16.5" customHeight="1">
-      <c r="A20" s="2"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="10"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="4"/>
     </row>
     <row r="21" ht="16.5" customHeight="1">
-      <c r="A21" s="2"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
     </row>
     <row r="22" ht="16.5" customHeight="1">
-      <c r="A22" s="2"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
     </row>
     <row r="23" ht="16.5" customHeight="1">
-      <c r="A23" s="2"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
     </row>
     <row r="24" ht="16.5" customHeight="1">
-      <c r="A24" s="2"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H13" r:id="rId1" location="" tooltip="" display=""/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>